<commit_message>
Add SetPropertyUsing overload that passes back the cell to the caller (fixes #79)
</commit_message>
<xml_diff>
--- a/ExcelMapper.Tests/ProductsConvert.xlsx
+++ b/ExcelMapper.Tests/ProductsConvert.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\ExcelMapper\ExcelMapper.Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A767DC-F921-410F-9646-0D2D3F2C8DF3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9B76FA-C5D5-4463-AB75-313B153B777A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,6 +84,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -100,7 +106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -108,6 +114,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -450,7 +457,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +513,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4">

</xml_diff>